<commit_message>
Updated Gantt Chart with testing
</commit_message>
<xml_diff>
--- a/BadWolf_Games_Gantt_Chart.xlsx
+++ b/BadWolf_Games_Gantt_Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
     <sheet name="Gantt Chart - Manual Duration" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>Start Date</t>
   </si>
@@ -188,12 +188,30 @@
   <si>
     <t>Add Second Level</t>
   </si>
+  <si>
+    <t>Can the enemies damage the player?</t>
+  </si>
+  <si>
+    <t>Can the player damage enemies?</t>
+  </si>
+  <si>
+    <t>Do the bosses damage enemies and visa versa?</t>
+  </si>
+  <si>
+    <t>Is movement fluid?</t>
+  </si>
+  <si>
+    <t>Crafting combinations work?</t>
+  </si>
+  <si>
+    <t>Weapon Transition are intuitive?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,6 +287,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -366,7 +390,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -434,6 +458,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,19 +492,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -2093,22 +2120,22 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>22.5</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>12.5</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.299999999999999</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.25</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -2117,7 +2144,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.9375</c:v>
+                  <c:v>11.700000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2585,22 +2612,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>12.5</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.7000000000000011</c:v>
+                  <c:v>1.8999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.75</c:v>
+                  <c:v>1.8999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>12</c:v>
@@ -2609,7 +2636,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0625</c:v>
+                  <c:v>0.29999999999999893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4391,7 +4418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4480,16 +4507,16 @@
         <f>C5</f>
         <v>42576</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="2:20" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
@@ -4845,34 +4872,34 @@
       <c r="G32" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="37" t="s">
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
+      <c r="P32" s="44"/>
     </row>
     <row r="33" spans="8:16" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H33" s="36" t="s">
+      <c r="H33" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36" t="s">
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="N33" s="36"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="36"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4890,12 +4917,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:V56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4916,24 +4943,24 @@
   <sheetData>
     <row r="1" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:22" ht="87" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
@@ -4990,15 +5017,15 @@
         <f>C5</f>
         <v>43133</v>
       </c>
-      <c r="M4" s="41" t="s">
+      <c r="M4" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
     </row>
     <row r="5" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
@@ -5158,106 +5185,106 @@
       </c>
     </row>
     <row r="11" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="36">
         <v>43141</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="37">
         <f t="shared" si="0"/>
         <v>43157</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="38">
         <v>16</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="39">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H11" s="47">
+      <c r="H11" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="36">
         <v>43141</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="37">
         <f t="shared" si="0"/>
         <v>43157</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="38">
         <v>16</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="39">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="47">
+      <c r="H12" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="36">
         <v>43141</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="37">
         <f t="shared" si="0"/>
         <v>43157</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="38">
         <v>16</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="39">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="47">
+      <c r="H13" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="36">
         <v>43141</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="37">
         <f t="shared" si="0"/>
         <v>43157</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="38">
         <v>16</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="39">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H14" s="47">
+      <c r="H14" s="40">
         <v>1</v>
       </c>
     </row>
@@ -5277,40 +5304,40 @@
       </c>
       <c r="F15" s="33">
         <f t="shared" ref="F15" si="4">IF(((D15)=""),"",(H15)*(D15-C15))</f>
-        <v>10</v>
+        <v>22.5</v>
       </c>
       <c r="G15" s="33">
         <f t="shared" ref="G15" si="5">IF(F15="","",(D15-C15)-F15)</f>
-        <v>15</v>
+        <v>2.5</v>
       </c>
       <c r="H15" s="34">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="16" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="36">
         <v>43157</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="37">
         <f t="shared" ref="D16" si="6">IF(ISBLANK(E16),"",E16+C16)</f>
         <v>43182</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="38">
         <v>25</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="39">
         <f t="shared" ref="F16" si="7">IF(((D16)=""),"",(H16)*(D16-C16))</f>
-        <v>22.5</v>
-      </c>
-      <c r="G16" s="33">
+        <v>25</v>
+      </c>
+      <c r="G16" s="39">
         <f t="shared" ref="G16" si="8">IF(F16="","",(D16-C16)-F16)</f>
-        <v>2.5</v>
-      </c>
-      <c r="H16" s="34">
-        <v>0.9</v>
+        <v>0</v>
+      </c>
+      <c r="H16" s="40">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5329,14 +5356,14 @@
       </c>
       <c r="F17" s="33">
         <f>IF(((D17)=""),"",(H17)*(D17-C17))</f>
-        <v>12.5</v>
+        <v>22.5</v>
       </c>
       <c r="G17" s="33">
         <f>IF(F17="","",(D17-C17)-F17)</f>
-        <v>12.5</v>
+        <v>2.5</v>
       </c>
       <c r="H17" s="34">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="J17" s="1"/>
     </row>
@@ -5367,14 +5394,14 @@
       </c>
       <c r="F19" s="17">
         <f>IF(((D19)=""),"",(H19)*(D19-C19))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G19" s="17">
         <f>IF(F19="","",(D19-C19)-F19)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H19" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5393,14 +5420,14 @@
       </c>
       <c r="F20" s="33">
         <f>IF(((D20)=""),"",(H20)*(D20-C20))</f>
-        <v>13.299999999999999</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="G20" s="33">
         <f>IF(F20="","",(D20-C20)-F20)</f>
-        <v>5.7000000000000011</v>
+        <v>1.8999999999999986</v>
       </c>
       <c r="H20" s="34">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5419,14 +5446,14 @@
       </c>
       <c r="F21" s="33">
         <f>IF(((D21)=""),"",(H21)*(D21-C21))</f>
-        <v>14.25</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="G21" s="33">
         <f>IF(F21="","",(D21-C21)-F21)</f>
-        <v>4.75</v>
+        <v>1.8999999999999986</v>
       </c>
       <c r="H21" s="34">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5508,24 +5535,48 @@
       </c>
       <c r="F25" s="17">
         <f>IF(((D25)=""),"",(H25)*(D25-C25))</f>
-        <v>9.9375</v>
+        <v>11.700000000000001</v>
       </c>
       <c r="G25" s="17">
         <f>IF(F25="","",(D25-C25)-F25)</f>
-        <v>2.0625</v>
+        <v>0.29999999999999893</v>
       </c>
       <c r="H25" s="23">
         <f>SUM(H5:H24)/16</f>
-        <v>0.828125</v>
+        <v>0.97500000000000009</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="49" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="33" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="11"/>
@@ -5538,18 +5589,18 @@
       <c r="J34" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K34" s="35" t="s">
+      <c r="K34" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="37" t="s">
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="Q34" s="37"/>
-      <c r="R34" s="37"/>
+      <c r="Q34" s="44"/>
+      <c r="R34" s="44"/>
     </row>
     <row r="35" spans="2:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="11"/>
@@ -5559,18 +5610,18 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="K35" s="36" t="s">
+      <c r="K35" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="36"/>
-      <c r="O35" s="36"/>
-      <c r="P35" s="36" t="s">
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="Q35" s="36"/>
-      <c r="R35" s="36"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="43"/>
     </row>
     <row r="36" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
@@ -5771,7 +5822,7 @@
     <mergeCell ref="P35:R35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>